<commit_message>
find and validad data
</commit_message>
<xml_diff>
--- a/excel-basic/excel_first/principiante2.xlsx
+++ b/excel-basic/excel_first/principiante2.xlsx
@@ -8,17 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\github\DataScience\excel-basic\excel_first\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794C3761-CD15-4CB0-A438-D39B0CAB73DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2A0375-A263-4E7E-AC90-1DE84EC966DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="240" windowWidth="20730" windowHeight="11400" activeTab="3" xr2:uid="{4A2F7486-93B3-460F-A0EB-8C08A45BB859}"/>
+    <workbookView xWindow="6960" yWindow="480" windowWidth="13320" windowHeight="10110" firstSheet="6" activeTab="7" xr2:uid="{4A2F7486-93B3-460F-A0EB-8C08A45BB859}"/>
   </bookViews>
   <sheets>
     <sheet name="6_funcionesBasic" sheetId="1" r:id="rId1"/>
     <sheet name="7_buscarV" sheetId="2" r:id="rId2"/>
     <sheet name="inv" sheetId="3" r:id="rId3"/>
     <sheet name="8_color" sheetId="4" r:id="rId4"/>
+    <sheet name="9_valData" sheetId="5" r:id="rId5"/>
+    <sheet name="10_grapDic" sheetId="8" r:id="rId6"/>
+    <sheet name="10_fechas" sheetId="11" r:id="rId7"/>
+    <sheet name="10_2table" sheetId="10" r:id="rId8"/>
+    <sheet name="10_FILT_TABLE" sheetId="6" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'10_FILT_TABLE'!$A$4:$H$20</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="43" r:id="rId10"/>
+    <pivotCache cacheId="53" r:id="rId11"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="97">
   <si>
     <t>CONOCIMIENTO PARA TODOS</t>
   </si>
@@ -187,6 +199,147 @@
   </si>
   <si>
     <t>Numero de Alumnos</t>
+  </si>
+  <si>
+    <t>BASE DE DATOS CLIENTES</t>
+  </si>
+  <si>
+    <t>DOCUMENTO</t>
+  </si>
+  <si>
+    <t>NOMBRES Y APELLIDOS</t>
+  </si>
+  <si>
+    <t>FECHA DE INGRESO</t>
+  </si>
+  <si>
+    <t>SEXO</t>
+  </si>
+  <si>
+    <t>CARGO</t>
+  </si>
+  <si>
+    <t>SUELDO BASICO</t>
+  </si>
+  <si>
+    <t>DIAS TRAB.</t>
+  </si>
+  <si>
+    <t>TOTAL SUELDO</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>INGENIERO</t>
+  </si>
+  <si>
+    <t>Dostin Hurtado</t>
+  </si>
+  <si>
+    <t>Sandy Olivera</t>
+  </si>
+  <si>
+    <t>Oscar Hurtado</t>
+  </si>
+  <si>
+    <t>Tatiana Aya</t>
+  </si>
+  <si>
+    <t>Luis Ramirez</t>
+  </si>
+  <si>
+    <t>Carlos Cedeno</t>
+  </si>
+  <si>
+    <t>Omar Corredor</t>
+  </si>
+  <si>
+    <t>Carlos Andres</t>
+  </si>
+  <si>
+    <t>Fuckencio Martines</t>
+  </si>
+  <si>
+    <t>Edgar Ortiz</t>
+  </si>
+  <si>
+    <t>Alberto Ochoa</t>
+  </si>
+  <si>
+    <t>Alejandro Guzman</t>
+  </si>
+  <si>
+    <t>Jenny Colmenarez</t>
+  </si>
+  <si>
+    <t>Nelsy Pico</t>
+  </si>
+  <si>
+    <t>Erika Herrera</t>
+  </si>
+  <si>
+    <t>Trollencio Gimenes</t>
+  </si>
+  <si>
+    <t>MASCULINO</t>
+  </si>
+  <si>
+    <t>FEMENINO</t>
+  </si>
+  <si>
+    <t>ORIENTADOR/A</t>
+  </si>
+  <si>
+    <t>SECRETARIA/O</t>
+  </si>
+  <si>
+    <t>ECONOMISTA</t>
+  </si>
+  <si>
+    <t>ABOGADO/A</t>
+  </si>
+  <si>
+    <t>GERENTE</t>
+  </si>
+  <si>
+    <t>Etiquetas de fila</t>
+  </si>
+  <si>
+    <t>Total general</t>
+  </si>
+  <si>
+    <t>Suma de TOTAL SUELDO</t>
+  </si>
+  <si>
+    <t>Suma de DIAS TRAB.</t>
+  </si>
+  <si>
+    <t>Suma de SUELDO BASICO</t>
+  </si>
+  <si>
+    <t>Florencia Gimenes</t>
+  </si>
+  <si>
+    <t>ago</t>
+  </si>
+  <si>
+    <t>sep</t>
+  </si>
+  <si>
+    <t>ene</t>
+  </si>
+  <si>
+    <t>oct</t>
+  </si>
+  <si>
+    <t>nov</t>
+  </si>
+  <si>
+    <t>dic</t>
   </si>
 </sst>
 </file>
@@ -199,7 +352,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +394,14 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -338,7 +499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -367,6 +528,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -394,11 +570,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -415,27 +588,56 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -488,6 +690,1887 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[principiante2.xlsx]10_grapDic!TablaDinámica2</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-GT"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-GT"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-GT"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'10_grapDic'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Suma de SUELDO BASICO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'10_grapDic'!$A$4:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Carlos Andres</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Erika Herrera</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Fuckencio Martines</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'10_grapDic'!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>300007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C0A6-4317-B2B2-4280244293AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'10_grapDic'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Suma de TOTAL SUELDO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'10_grapDic'!$A$4:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Carlos Andres</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Erika Herrera</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Fuckencio Martines</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'10_grapDic'!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>300007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>260012.13333333336</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>140003.73333333334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C0A6-4317-B2B2-4280244293AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:shape val="box"/>
+        <c:axId val="1683449247"/>
+        <c:axId val="1823832671"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="1683449247"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1823832671"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1823832671"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1683449247"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-GT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-GT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94E18F0A-B3FE-4B89-9642-81288319623D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="USUARIO" refreshedDate="45155.038824537034" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="17" xr:uid="{E5A7D6FB-B0F4-4963-AB1C-5420FE364460}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A4:H21" sheet="10_FILT_TABLE"/>
+  </cacheSource>
+  <cacheFields count="8">
+    <cacheField name="DOCUMENTO" numFmtId="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1121885" maxValue="1121901"/>
+    </cacheField>
+    <cacheField name="NOMBRES Y APELLIDOS" numFmtId="0">
+      <sharedItems count="17">
+        <s v="Dostin Hurtado"/>
+        <s v="Sandy Olivera"/>
+        <s v="Oscar Hurtado"/>
+        <s v="Tatiana Aya"/>
+        <s v="Luis Ramirez"/>
+        <s v="Carlos Cedeno"/>
+        <s v="Omar Corredor"/>
+        <s v="Carlos Andres"/>
+        <s v="Fuckencio Martines"/>
+        <s v="Edgar Ortiz"/>
+        <s v="Alberto Ochoa"/>
+        <s v="Alejandro Guzman"/>
+        <s v="Jenny Colmenarez"/>
+        <s v="Nelsy Pico"/>
+        <s v="Erika Herrera"/>
+        <s v="Trollencio Gimenes"/>
+        <s v="Florencia Gimenes"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="FECHA DE INGRESO" numFmtId="14">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="SEXO" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="CARGO" numFmtId="0">
+      <sharedItems count="6">
+        <s v="INGENIERO"/>
+        <s v="ORIENTADOR/A"/>
+        <s v="SECRETARIA/O"/>
+        <s v="ECONOMISTA"/>
+        <s v="ABOGADO/A"/>
+        <s v="GERENTE"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="SUELDO BASICO" numFmtId="165">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="300001" maxValue="6000000"/>
+    </cacheField>
+    <cacheField name="DIAS TRAB." numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="10" maxValue="30"/>
+    </cacheField>
+    <cacheField name="TOTAL SUELDO" numFmtId="165">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="100002" maxValue="3000000"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="USUARIO" refreshedDate="45155.04483136574" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="17" xr:uid="{F4A88920-A2EC-4219-B055-B02677B8D023}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A4:H21" sheet="10_2table"/>
+  </cacheSource>
+  <cacheFields count="8">
+    <cacheField name="DOCUMENTO" numFmtId="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1121885" maxValue="1121901"/>
+    </cacheField>
+    <cacheField name="NOMBRES Y APELLIDOS" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="FECHA DE INGRESO" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2023-08-16T00:00:00" maxDate="2024-01-02T00:00:00" count="17">
+        <d v="2023-08-16T00:00:00"/>
+        <d v="2023-08-17T00:00:00"/>
+        <d v="2023-08-18T00:00:00"/>
+        <d v="2023-09-19T00:00:00"/>
+        <d v="2023-09-20T00:00:00"/>
+        <d v="2023-09-21T00:00:00"/>
+        <d v="2023-09-22T00:00:00"/>
+        <d v="2023-09-23T00:00:00"/>
+        <d v="2023-10-24T00:00:00"/>
+        <d v="2023-10-25T00:00:00"/>
+        <d v="2023-10-26T00:00:00"/>
+        <d v="2023-10-27T00:00:00"/>
+        <d v="2023-11-28T00:00:00"/>
+        <d v="2023-11-29T00:00:00"/>
+        <d v="2023-12-30T00:00:00"/>
+        <d v="2023-12-31T00:00:00"/>
+        <d v="2024-01-01T00:00:00"/>
+      </sharedItems>
+      <fieldGroup base="2">
+        <rangePr groupBy="months" startDate="2023-08-16T00:00:00" endDate="2024-01-02T00:00:00"/>
+        <groupItems count="14">
+          <s v="&lt;16/08/2023"/>
+          <s v="ene"/>
+          <s v="feb"/>
+          <s v="mar"/>
+          <s v="abr"/>
+          <s v="may"/>
+          <s v="jun"/>
+          <s v="jul"/>
+          <s v="ago"/>
+          <s v="sep"/>
+          <s v="oct"/>
+          <s v="nov"/>
+          <s v="dic"/>
+          <s v="&gt;02/01/2024"/>
+        </groupItems>
+      </fieldGroup>
+    </cacheField>
+    <cacheField name="SEXO" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="CARGO" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="SUELDO BASICO" numFmtId="165">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="300001" maxValue="6000000"/>
+    </cacheField>
+    <cacheField name="DIAS TRAB." numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="10" maxValue="30"/>
+    </cacheField>
+    <cacheField name="TOTAL SUELDO" numFmtId="165">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="100002" maxValue="3000000"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="17">
+  <r>
+    <n v="1121885"/>
+    <x v="0"/>
+    <m/>
+    <s v="MASCULINO"/>
+    <x v="0"/>
+    <n v="6000000"/>
+    <n v="15"/>
+    <n v="3000000"/>
+  </r>
+  <r>
+    <n v="1121886"/>
+    <x v="1"/>
+    <m/>
+    <s v="FEMENINO"/>
+    <x v="1"/>
+    <n v="300001"/>
+    <n v="18"/>
+    <n v="180000.59999999998"/>
+  </r>
+  <r>
+    <n v="1121887"/>
+    <x v="2"/>
+    <m/>
+    <s v="MASCULINO"/>
+    <x v="1"/>
+    <n v="300002"/>
+    <n v="19"/>
+    <n v="190001.26666666669"/>
+  </r>
+  <r>
+    <n v="1121888"/>
+    <x v="3"/>
+    <m/>
+    <s v="FEMENINO"/>
+    <x v="2"/>
+    <n v="300003"/>
+    <n v="28"/>
+    <n v="280002.8"/>
+  </r>
+  <r>
+    <n v="1121889"/>
+    <x v="4"/>
+    <m/>
+    <s v="MASCULINO"/>
+    <x v="3"/>
+    <n v="300004"/>
+    <n v="15"/>
+    <n v="150002"/>
+  </r>
+  <r>
+    <n v="1121890"/>
+    <x v="5"/>
+    <m/>
+    <s v="MASCULINO"/>
+    <x v="3"/>
+    <n v="300005"/>
+    <n v="25"/>
+    <n v="250004.16666666666"/>
+  </r>
+  <r>
+    <n v="1121891"/>
+    <x v="6"/>
+    <m/>
+    <s v="MASCULINO"/>
+    <x v="0"/>
+    <n v="300006"/>
+    <n v="10"/>
+    <n v="100002"/>
+  </r>
+  <r>
+    <n v="1121892"/>
+    <x v="7"/>
+    <m/>
+    <s v="MASCULINO"/>
+    <x v="4"/>
+    <n v="300007"/>
+    <n v="30"/>
+    <n v="300007"/>
+  </r>
+  <r>
+    <n v="1121893"/>
+    <x v="8"/>
+    <m/>
+    <s v="MASCULINO"/>
+    <x v="4"/>
+    <n v="300008"/>
+    <n v="14"/>
+    <n v="140003.73333333334"/>
+  </r>
+  <r>
+    <n v="1121894"/>
+    <x v="9"/>
+    <m/>
+    <s v="MASCULINO"/>
+    <x v="5"/>
+    <n v="300009"/>
+    <n v="16"/>
+    <n v="160004.79999999999"/>
+  </r>
+  <r>
+    <n v="1121895"/>
+    <x v="10"/>
+    <m/>
+    <s v="MASCULINO"/>
+    <x v="5"/>
+    <n v="300010"/>
+    <n v="18"/>
+    <n v="180006"/>
+  </r>
+  <r>
+    <n v="1121896"/>
+    <x v="11"/>
+    <m/>
+    <s v="MASCULINO"/>
+    <x v="2"/>
+    <n v="300011"/>
+    <n v="20"/>
+    <n v="200007.33333333334"/>
+  </r>
+  <r>
+    <n v="1121897"/>
+    <x v="12"/>
+    <m/>
+    <s v="FEMENINO"/>
+    <x v="2"/>
+    <n v="300012"/>
+    <n v="22"/>
+    <n v="220008.8"/>
+  </r>
+  <r>
+    <n v="1121898"/>
+    <x v="13"/>
+    <m/>
+    <s v="FEMENINO"/>
+    <x v="2"/>
+    <n v="300013"/>
+    <n v="24"/>
+    <n v="240010.39999999997"/>
+  </r>
+  <r>
+    <n v="1121899"/>
+    <x v="14"/>
+    <m/>
+    <s v="FEMENINO"/>
+    <x v="4"/>
+    <n v="300014"/>
+    <n v="26"/>
+    <n v="260012.13333333336"/>
+  </r>
+  <r>
+    <n v="1121900"/>
+    <x v="15"/>
+    <m/>
+    <s v="MASCULINO"/>
+    <x v="0"/>
+    <n v="1300015"/>
+    <n v="30"/>
+    <n v="1300015"/>
+  </r>
+  <r>
+    <n v="1121901"/>
+    <x v="16"/>
+    <m/>
+    <s v="FEMENINO"/>
+    <x v="3"/>
+    <n v="1300015"/>
+    <n v="18"/>
+    <n v="780009"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="17">
+  <r>
+    <n v="1121885"/>
+    <s v="Dostin Hurtado"/>
+    <x v="0"/>
+    <s v="MASCULINO"/>
+    <s v="INGENIERO"/>
+    <n v="6000000"/>
+    <n v="15"/>
+    <n v="3000000"/>
+  </r>
+  <r>
+    <n v="1121886"/>
+    <s v="Sandy Olivera"/>
+    <x v="1"/>
+    <s v="FEMENINO"/>
+    <s v="ORIENTADOR/A"/>
+    <n v="300001"/>
+    <n v="18"/>
+    <n v="180000.59999999998"/>
+  </r>
+  <r>
+    <n v="1121887"/>
+    <s v="Oscar Hurtado"/>
+    <x v="2"/>
+    <s v="MASCULINO"/>
+    <s v="ORIENTADOR/A"/>
+    <n v="300002"/>
+    <n v="19"/>
+    <n v="190001.26666666669"/>
+  </r>
+  <r>
+    <n v="1121888"/>
+    <s v="Tatiana Aya"/>
+    <x v="3"/>
+    <s v="FEMENINO"/>
+    <s v="SECRETARIA/O"/>
+    <n v="300003"/>
+    <n v="28"/>
+    <n v="280002.8"/>
+  </r>
+  <r>
+    <n v="1121889"/>
+    <s v="Luis Ramirez"/>
+    <x v="4"/>
+    <s v="MASCULINO"/>
+    <s v="ECONOMISTA"/>
+    <n v="300004"/>
+    <n v="15"/>
+    <n v="150002"/>
+  </r>
+  <r>
+    <n v="1121890"/>
+    <s v="Carlos Cedeno"/>
+    <x v="5"/>
+    <s v="MASCULINO"/>
+    <s v="ECONOMISTA"/>
+    <n v="300005"/>
+    <n v="25"/>
+    <n v="250004.16666666666"/>
+  </r>
+  <r>
+    <n v="1121891"/>
+    <s v="Omar Corredor"/>
+    <x v="6"/>
+    <s v="MASCULINO"/>
+    <s v="INGENIERO"/>
+    <n v="300006"/>
+    <n v="10"/>
+    <n v="100002"/>
+  </r>
+  <r>
+    <n v="1121892"/>
+    <s v="Carlos Andres"/>
+    <x v="7"/>
+    <s v="MASCULINO"/>
+    <s v="ABOGADO/A"/>
+    <n v="300007"/>
+    <n v="30"/>
+    <n v="300007"/>
+  </r>
+  <r>
+    <n v="1121893"/>
+    <s v="Fuckencio Martines"/>
+    <x v="8"/>
+    <s v="MASCULINO"/>
+    <s v="ABOGADO/A"/>
+    <n v="300008"/>
+    <n v="14"/>
+    <n v="140003.73333333334"/>
+  </r>
+  <r>
+    <n v="1121894"/>
+    <s v="Edgar Ortiz"/>
+    <x v="9"/>
+    <s v="MASCULINO"/>
+    <s v="GERENTE"/>
+    <n v="300009"/>
+    <n v="16"/>
+    <n v="160004.79999999999"/>
+  </r>
+  <r>
+    <n v="1121895"/>
+    <s v="Alberto Ochoa"/>
+    <x v="10"/>
+    <s v="MASCULINO"/>
+    <s v="GERENTE"/>
+    <n v="300010"/>
+    <n v="18"/>
+    <n v="180006"/>
+  </r>
+  <r>
+    <n v="1121896"/>
+    <s v="Alejandro Guzman"/>
+    <x v="11"/>
+    <s v="MASCULINO"/>
+    <s v="SECRETARIA/O"/>
+    <n v="300011"/>
+    <n v="20"/>
+    <n v="200007.33333333334"/>
+  </r>
+  <r>
+    <n v="1121897"/>
+    <s v="Jenny Colmenarez"/>
+    <x v="12"/>
+    <s v="FEMENINO"/>
+    <s v="SECRETARIA/O"/>
+    <n v="300012"/>
+    <n v="22"/>
+    <n v="220008.8"/>
+  </r>
+  <r>
+    <n v="1121898"/>
+    <s v="Nelsy Pico"/>
+    <x v="13"/>
+    <s v="FEMENINO"/>
+    <s v="SECRETARIA/O"/>
+    <n v="300013"/>
+    <n v="24"/>
+    <n v="240010.39999999997"/>
+  </r>
+  <r>
+    <n v="1121899"/>
+    <s v="Erika Herrera"/>
+    <x v="14"/>
+    <s v="FEMENINO"/>
+    <s v="ABOGADO/A"/>
+    <n v="300014"/>
+    <n v="26"/>
+    <n v="260012.13333333336"/>
+  </r>
+  <r>
+    <n v="1121900"/>
+    <s v="Trollencio Gimenes"/>
+    <x v="15"/>
+    <s v="MASCULINO"/>
+    <s v="INGENIERO"/>
+    <n v="1300015"/>
+    <n v="30"/>
+    <n v="1300015"/>
+  </r>
+  <r>
+    <n v="1121901"/>
+    <s v="Florencia Gimenes"/>
+    <x v="16"/>
+    <s v="FEMENINO"/>
+    <s v="ECONOMISTA"/>
+    <n v="1300015"/>
+    <n v="18"/>
+    <n v="780009"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{21E26E1D-868A-4BCC-AE36-503A12869181}" name="TablaDinámica2" cacheId="43" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:C7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="8">
+    <pivotField numFmtId="3" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="18">
+        <item x="10"/>
+        <item x="11"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="9"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="12"/>
+        <item x="4"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="7">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="165" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="165" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="4" item="0" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Suma de SUELDO BASICO" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Suma de TOTAL SUELDO" fld="7" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="7">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{222A12BF-BC6D-4432-89AF-AD1CDEC31B9F}" name="TablaDinámica3" cacheId="53" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:D10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField numFmtId="3" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" numFmtId="14" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="165" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="165" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="3">
+    <dataField name="Suma de SUELDO BASICO" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Suma de DIAS TRAB." fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Suma de TOTAL SUELDO" fld="7" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="6">
+            <x v="1"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -800,26 +2883,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -945,97 +3028,97 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="17"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="14"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="5">
         <f>MAX(F6:F9)</f>
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="14"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="5">
         <f>MIN(F6:F9)</f>
         <v>5.333333333333333</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="14"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="5">
         <f>IFERROR(MODE(F6:F9),"Ninguna")</f>
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="14"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="5">
         <f>AVERAGE(F6:F9)</f>
         <v>7.333333333333333</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="14"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="8">
         <f>COUNTA(F6:F10)</f>
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="14"/>
+      <c r="D18" s="19"/>
       <c r="E18" s="8">
         <f>COUNTIF(G6:G9,"Aprobado")</f>
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="14"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="8">
         <f>COUNTIF(G6:G9,"Reprobado")</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="14"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="5">
         <f>AVERAGEIF(G6:G9,"Aprobado",F6:F9)</f>
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="14"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="5">
         <f>AVERAGEIF(G6:G9,"Reprobado",F6:F9)</f>
         <v>5.333333333333333</v>
@@ -1043,11 +3126,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C17:D17"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="A3:G3"/>
@@ -1055,6 +3133,11 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C17:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1076,20 +3159,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
@@ -1210,11 +3293,11 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
       <c r="E12" s="13">
         <f>SUM(E7:E11)</f>
         <v>18000</v>
@@ -1243,16 +3326,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -1365,8 +3448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE18BDC9-454B-4E4B-B1E0-710A3708D7C2}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,26 +3459,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1529,112 +3612,119 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="17"/>
-      <c r="G12" s="24" t="s">
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
+      <c r="G12" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="24"/>
+      <c r="H12" s="34"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="31">
+      <c r="D13" s="19"/>
+      <c r="E13" s="15">
         <f>MAX(F6:F9)</f>
         <v>5</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="35">
         <v>3</v>
       </c>
-      <c r="H13" s="23"/>
+      <c r="H13" s="35"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="31">
+      <c r="D14" s="19"/>
+      <c r="E14" s="15">
         <f>MIN(F6:F9)</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="31">
+      <c r="D15" s="19"/>
+      <c r="E15" s="15">
         <f>AVERAGE(F6:F9)</f>
         <v>2.9166666666666665</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="32">
+      <c r="D16" s="29"/>
+      <c r="E16" s="16">
         <f>COUNTIF(G6:G9,"EXCELENTE")</f>
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="33">
+      <c r="D17" s="31"/>
+      <c r="E17" s="17">
         <f>COUNTIF(G6:G9,"SOBRESALIENTE")</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="32">
+      <c r="D18" s="29"/>
+      <c r="E18" s="16">
         <f>COUNTIF(G6:G9,"ACEPTABLE")</f>
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="29"/>
-      <c r="E19" s="32">
+      <c r="D19" s="33"/>
+      <c r="E19" s="16">
         <f>COUNTIF(G6:G9,"INSUFICIENTE")</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="29"/>
-      <c r="E20" s="32">
+      <c r="D20" s="33"/>
+      <c r="E20" s="16">
         <f>COUNTIF(G6:G9,"DEFICIENTE")</f>
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="34">
+      <c r="D21" s="28"/>
+      <c r="E21" s="18">
         <f>COUNTA(F6:F9)</f>
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
@@ -1642,13 +3732,6 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F9">
     <cfRule type="iconSet" priority="6">
@@ -1660,23 +3743,1556 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G9">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="DEFICIENTE">
+    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="DEFICIENTE">
       <formula>NOT(ISERROR(SEARCH("DEFICIENTE",G6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="INSUFICIENTE">
+    <cfRule type="containsText" dxfId="11" priority="2" operator="containsText" text="INSUFICIENTE">
       <formula>NOT(ISERROR(SEARCH("INSUFICIENTE",G6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="ACEPTABLE">
+    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="ACEPTABLE">
       <formula>NOT(ISERROR(SEARCH("ACEPTABLE",G6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="SOBRESALIENTE">
+    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="SOBRESALIENTE">
       <formula>NOT(ISERROR(SEARCH("SOBRESALIENTE",G6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="EXCELENTE">
+    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="EXCELENTE">
       <formula>NOT(ISERROR(SEARCH("EXCELENTE",G6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D032EF-655B-401E-BB41-523F5C9FA9A7}">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection sqref="A1:H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="37">
+        <v>45152</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <dataValidations count="5">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="Solo se admiten entre 5 y 20 caracteres." promptTitle="Cuidado" prompt="Nombre entre 5 y 20 letras" sqref="B5" xr:uid="{C5C23880-33BB-4F7C-87AC-AF27C6F44342}">
+      <formula1>5</formula1>
+      <formula2>20</formula2>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{84E8B5F6-B99F-4092-B4C9-E81D0C543D98}">
+      <formula1>45151</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5" xr:uid="{EE986A23-0E84-4872-8039-CE427691EB87}">
+      <formula1>"Masculino, Femenino, Otro"</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5" xr:uid="{0F157139-16EA-4B9F-9A53-1CD24D5FD143}">
+      <formula1>10</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5" xr:uid="{5AE1765B-50B1-47E0-A1C8-30D6E9F2F850}">
+      <formula1>EXACT(UPPER(E5),E5)</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3EC54FF-13DA-438A-AD3C-3D127A4400C7}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="42">
+        <v>300007</v>
+      </c>
+      <c r="C4" s="42">
+        <v>300007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="42">
+        <v>300014</v>
+      </c>
+      <c r="C5" s="42">
+        <v>260012.13333333336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="42">
+        <v>300008</v>
+      </c>
+      <c r="C6" s="42">
+        <v>140003.73333333334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="42">
+        <v>900029</v>
+      </c>
+      <c r="C7" s="42">
+        <v>700022.8666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2257DD66-3212-4890-A1E1-4C407ABC84CC}">
+  <dimension ref="A3:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="42">
+        <v>1300015</v>
+      </c>
+      <c r="C4" s="42">
+        <v>18</v>
+      </c>
+      <c r="D4" s="42">
+        <v>780009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="42">
+        <v>6600003</v>
+      </c>
+      <c r="C5" s="42">
+        <v>52</v>
+      </c>
+      <c r="D5" s="42">
+        <v>3370001.8666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="42">
+        <v>1500025</v>
+      </c>
+      <c r="C6" s="42">
+        <v>108</v>
+      </c>
+      <c r="D6" s="42">
+        <v>1080017.9666666668</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="42">
+        <v>1200038</v>
+      </c>
+      <c r="C7" s="42">
+        <v>68</v>
+      </c>
+      <c r="D7" s="42">
+        <v>680021.8666666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="42">
+        <v>600025</v>
+      </c>
+      <c r="C8" s="42">
+        <v>46</v>
+      </c>
+      <c r="D8" s="42">
+        <v>460019.19999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="42">
+        <v>1600029</v>
+      </c>
+      <c r="C9" s="42">
+        <v>56</v>
+      </c>
+      <c r="D9" s="42">
+        <v>1560027.1333333333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="39">
+        <v>12800135</v>
+      </c>
+      <c r="C10" s="39">
+        <v>348</v>
+      </c>
+      <c r="D10" s="39">
+        <v>7930097.0333333351</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE39B69-C4C4-4516-9561-EEB81F46E438}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="38">
+        <v>1121885</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="37">
+        <v>45154</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="3">
+        <v>6000000</v>
+      </c>
+      <c r="G5" s="1">
+        <v>15</v>
+      </c>
+      <c r="H5" s="3">
+        <f>F5/30*G5</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="38">
+        <v>1121886</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="37">
+        <v>45155</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="3">
+        <v>300001</v>
+      </c>
+      <c r="G6" s="1">
+        <v>18</v>
+      </c>
+      <c r="H6" s="3">
+        <f t="shared" ref="H6:H21" si="0">F6/30*G6</f>
+        <v>180000.59999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="38">
+        <v>1121887</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="37">
+        <v>45156</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="3">
+        <v>300002</v>
+      </c>
+      <c r="G7" s="1">
+        <v>19</v>
+      </c>
+      <c r="H7" s="3">
+        <f t="shared" si="0"/>
+        <v>190001.26666666669</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="38">
+        <v>1121888</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="37">
+        <v>45188</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="3">
+        <v>300003</v>
+      </c>
+      <c r="G8" s="1">
+        <v>28</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" si="0"/>
+        <v>280002.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="38">
+        <v>1121889</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="37">
+        <v>45189</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="3">
+        <v>300004</v>
+      </c>
+      <c r="G9" s="1">
+        <v>15</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="0"/>
+        <v>150002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="38">
+        <v>1121890</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="37">
+        <v>45190</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="3">
+        <v>300005</v>
+      </c>
+      <c r="G10" s="1">
+        <v>25</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="0"/>
+        <v>250004.16666666666</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="38">
+        <v>1121891</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="37">
+        <v>45191</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="3">
+        <v>300006</v>
+      </c>
+      <c r="G11" s="1">
+        <v>10</v>
+      </c>
+      <c r="H11" s="3">
+        <f t="shared" si="0"/>
+        <v>100002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="38">
+        <v>1121892</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="37">
+        <v>45192</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="3">
+        <v>300007</v>
+      </c>
+      <c r="G12" s="1">
+        <v>30</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" si="0"/>
+        <v>300007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="38">
+        <v>1121893</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="37">
+        <v>45223</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="3">
+        <v>300008</v>
+      </c>
+      <c r="G13" s="1">
+        <v>14</v>
+      </c>
+      <c r="H13" s="3">
+        <f t="shared" si="0"/>
+        <v>140003.73333333334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="38">
+        <v>1121894</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="37">
+        <v>45224</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="3">
+        <v>300009</v>
+      </c>
+      <c r="G14" s="1">
+        <v>16</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" si="0"/>
+        <v>160004.79999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="38">
+        <v>1121895</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="37">
+        <v>45225</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="3">
+        <v>300010</v>
+      </c>
+      <c r="G15" s="1">
+        <v>18</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" si="0"/>
+        <v>180006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="38">
+        <v>1121896</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="37">
+        <v>45226</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="3">
+        <v>300011</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="0"/>
+        <v>200007.33333333334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="38">
+        <v>1121897</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="37">
+        <v>45258</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="3">
+        <v>300012</v>
+      </c>
+      <c r="G17" s="1">
+        <v>22</v>
+      </c>
+      <c r="H17" s="3">
+        <f t="shared" si="0"/>
+        <v>220008.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="38">
+        <v>1121898</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="37">
+        <v>45259</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="3">
+        <v>300013</v>
+      </c>
+      <c r="G18" s="1">
+        <v>24</v>
+      </c>
+      <c r="H18" s="3">
+        <f t="shared" si="0"/>
+        <v>240010.39999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="38">
+        <v>1121899</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="37">
+        <v>45290</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="3">
+        <v>300014</v>
+      </c>
+      <c r="G19" s="1">
+        <v>26</v>
+      </c>
+      <c r="H19" s="3">
+        <f t="shared" si="0"/>
+        <v>260012.13333333336</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="38">
+        <v>1121900</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="37">
+        <v>45291</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1300015</v>
+      </c>
+      <c r="G20" s="1">
+        <v>30</v>
+      </c>
+      <c r="H20" s="3">
+        <f t="shared" si="0"/>
+        <v>1300015</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="38">
+        <v>1121901</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="37">
+        <v>45292</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1300015</v>
+      </c>
+      <c r="G21" s="1">
+        <v>18</v>
+      </c>
+      <c r="H21" s="3">
+        <f t="shared" si="0"/>
+        <v>780009</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <dataValidations count="6">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G21" xr:uid="{A617848D-0EC8-495D-935C-128BC34990EF}">
+      <formula1>1</formula1>
+      <formula2>31</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F21" xr:uid="{99CAB2A4-2D26-4BED-9B83-3F2DFA3F0603}">
+      <formula1>299999</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D21" xr:uid="{235BAE66-22CC-4A19-9462-EF3664A684B8}">
+      <formula1>"MASCULINO,FEMENINO,OTRO"</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="Solo se admiten entre 5 y 20 caracteres." promptTitle="Cuidado" prompt="Nombre entre 5 y 20 letras" sqref="B5:B21" xr:uid="{50D41330-22DF-4CEA-AE0C-3D83B16522D0}">
+      <formula1>5</formula1>
+      <formula2>20</formula2>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C21" xr:uid="{FF952961-6B13-4327-8E23-329F46631E9A}">
+      <formula1>45151</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E21" xr:uid="{CF6139A2-C4E7-4350-8146-A66AB4528A5F}">
+      <formula1>EXACT(UPPER(E5),E5)</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8120DAE1-299A-48BB-9702-11E16622D153}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView topLeftCell="D4" workbookViewId="0">
+      <selection sqref="A1:H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="38">
+        <v>1121885</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="37"/>
+      <c r="D5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="3">
+        <v>6000000</v>
+      </c>
+      <c r="G5" s="1">
+        <v>15</v>
+      </c>
+      <c r="H5" s="3">
+        <f>F5/30*G5</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="38">
+        <v>1121886</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="37"/>
+      <c r="D6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="3">
+        <v>300001</v>
+      </c>
+      <c r="G6" s="1">
+        <v>18</v>
+      </c>
+      <c r="H6" s="3">
+        <f t="shared" ref="H6:H21" si="0">F6/30*G6</f>
+        <v>180000.59999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="38">
+        <v>1121887</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="37"/>
+      <c r="D7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="3">
+        <v>300002</v>
+      </c>
+      <c r="G7" s="1">
+        <v>19</v>
+      </c>
+      <c r="H7" s="3">
+        <f t="shared" si="0"/>
+        <v>190001.26666666669</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="38">
+        <v>1121888</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="37"/>
+      <c r="D8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="3">
+        <v>300003</v>
+      </c>
+      <c r="G8" s="1">
+        <v>28</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" si="0"/>
+        <v>280002.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="38">
+        <v>1121889</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="37"/>
+      <c r="D9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="3">
+        <v>300004</v>
+      </c>
+      <c r="G9" s="1">
+        <v>15</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="0"/>
+        <v>150002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="38">
+        <v>1121890</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="3">
+        <v>300005</v>
+      </c>
+      <c r="G10" s="1">
+        <v>25</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="0"/>
+        <v>250004.16666666666</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="38">
+        <v>1121891</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="37"/>
+      <c r="D11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="3">
+        <v>300006</v>
+      </c>
+      <c r="G11" s="1">
+        <v>10</v>
+      </c>
+      <c r="H11" s="3">
+        <f t="shared" si="0"/>
+        <v>100002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="38">
+        <v>1121892</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="3">
+        <v>300007</v>
+      </c>
+      <c r="G12" s="1">
+        <v>30</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" si="0"/>
+        <v>300007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="38">
+        <v>1121893</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="37"/>
+      <c r="D13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="3">
+        <v>300008</v>
+      </c>
+      <c r="G13" s="1">
+        <v>14</v>
+      </c>
+      <c r="H13" s="3">
+        <f t="shared" si="0"/>
+        <v>140003.73333333334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="38">
+        <v>1121894</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="3">
+        <v>300009</v>
+      </c>
+      <c r="G14" s="1">
+        <v>16</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" si="0"/>
+        <v>160004.79999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="38">
+        <v>1121895</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="37"/>
+      <c r="D15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="3">
+        <v>300010</v>
+      </c>
+      <c r="G15" s="1">
+        <v>18</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" si="0"/>
+        <v>180006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="38">
+        <v>1121896</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="37"/>
+      <c r="D16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="3">
+        <v>300011</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="0"/>
+        <v>200007.33333333334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="38">
+        <v>1121897</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="37"/>
+      <c r="D17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="3">
+        <v>300012</v>
+      </c>
+      <c r="G17" s="1">
+        <v>22</v>
+      </c>
+      <c r="H17" s="3">
+        <f t="shared" si="0"/>
+        <v>220008.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="38">
+        <v>1121898</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="37"/>
+      <c r="D18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="3">
+        <v>300013</v>
+      </c>
+      <c r="G18" s="1">
+        <v>24</v>
+      </c>
+      <c r="H18" s="3">
+        <f t="shared" si="0"/>
+        <v>240010.39999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="38">
+        <v>1121899</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="37"/>
+      <c r="D19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="3">
+        <v>300014</v>
+      </c>
+      <c r="G19" s="1">
+        <v>26</v>
+      </c>
+      <c r="H19" s="3">
+        <f t="shared" si="0"/>
+        <v>260012.13333333336</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="38">
+        <v>1121900</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="37"/>
+      <c r="D20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1300015</v>
+      </c>
+      <c r="G20" s="1">
+        <v>30</v>
+      </c>
+      <c r="H20" s="3">
+        <f t="shared" si="0"/>
+        <v>1300015</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="38">
+        <v>1121901</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="37"/>
+      <c r="D21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1300015</v>
+      </c>
+      <c r="G21" s="1">
+        <v>18</v>
+      </c>
+      <c r="H21" s="3">
+        <f t="shared" si="0"/>
+        <v>780009</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A4:H20" xr:uid="{8120DAE1-299A-48BB-9702-11E16622D153}"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <dataValidations count="6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E21" xr:uid="{07242829-45FA-4755-97FB-DE465152B5B8}">
+      <formula1>EXACT(UPPER(E5),E5)</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C21" xr:uid="{092A1698-317F-461E-A93D-E203856EDDE1}">
+      <formula1>45151</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="Solo se admiten entre 5 y 20 caracteres." promptTitle="Cuidado" prompt="Nombre entre 5 y 20 letras" sqref="B5:B21" xr:uid="{386F2322-AD9D-4BE2-955F-D1DDD7FF5DEE}">
+      <formula1>5</formula1>
+      <formula2>20</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D21" xr:uid="{7723664C-AD55-4E86-B009-2DD0159EBD07}">
+      <formula1>"MASCULINO,FEMENINO,OTRO"</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F21" xr:uid="{F6C5FC56-9E1F-48B0-868D-680C8788EA5D}">
+      <formula1>299999</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G21" xr:uid="{0CAF318E-3052-48F7-96C9-3F5AF0300933}">
+      <formula1>1</formula1>
+      <formula2>31</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>